<commit_message>
updated reg and Pi
</commit_message>
<xml_diff>
--- a/Examples/multi_enzyme_model_regeneration.xlsx
+++ b/Examples/multi_enzyme_model_regeneration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dex36\Documents\GitHub\ODBM\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23618C-5CEC-4AC8-8858-0C1DA9739E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A2E82D-A8C6-4A3C-B034-3E3D6BEA2BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
   </bookViews>
@@ -434,7 +434,7 @@
     <t>Pi+</t>
   </si>
   <si>
-    <t>MMA</t>
+    <t>MMA; SPI</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1358,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C28"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>